<commit_message>
intermediate commit # atleast now
</commit_message>
<xml_diff>
--- a/Projects/LIONNZ/Data/Template.xlsx
+++ b/Projects/LIONNZ/Data/Template.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="67">
   <si>
     <t xml:space="preserve">kpi_name</t>
   </si>
@@ -30,6 +30,9 @@
     <t xml:space="preserve">kpi_family</t>
   </si>
   <si>
+    <t xml:space="preserve">active</t>
+  </si>
+  <si>
     <t xml:space="preserve">FSOS_OWN_MAN_ALL_SCENETYPE</t>
   </si>
   <si>
@@ -45,6 +48,9 @@
     <t xml:space="preserve">FSOS_ALL_MAN_ALL_SCENETYPE_ALL_BRAND_ALL_SKU</t>
   </si>
   <si>
+    <t xml:space="preserve">Add necessary scene types in details sheet</t>
+  </si>
+  <si>
     <t xml:space="preserve">FSOS_OWN_MAN_ALL_SUBCAT</t>
   </si>
   <si>
@@ -102,12 +108,15 @@
     <t xml:space="preserve">COUNT_SKU_FACINGS_BEER_TAP_CATEGORY_OWN_MANUFACTURER</t>
   </si>
   <si>
-    <t xml:space="preserve">Presence</t>
+    <t xml:space="preserve">Count</t>
   </si>
   <si>
     <t xml:space="preserve">COUNT_SKU_FACINGS_BEER_TAP_CATEGORY_ALL_MANUFACTURER</t>
   </si>
   <si>
+    <t xml:space="preserve">kpi_parent</t>
+  </si>
+  <si>
     <t xml:space="preserve">param_1</t>
   </si>
   <si>
@@ -132,30 +141,27 @@
     <t xml:space="preserve">param_4_value</t>
   </si>
   <si>
+    <t xml:space="preserve">numerator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">denominator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store_policy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">context</t>
+  </si>
+  <si>
+    <t xml:space="preserve">output</t>
+  </si>
+  <si>
+    <t xml:space="preserve">manufacturer</t>
+  </si>
+  <si>
     <t xml:space="preserve">scene_type</t>
   </si>
   <si>
-    <t xml:space="preserve">Numerator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Denominator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Store Policy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Context</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Output</t>
-  </si>
-  <si>
-    <t xml:space="preserve">manufacturer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Store</t>
-  </si>
-  <si>
     <t xml:space="preserve">lion</t>
   </si>
   <si>
@@ -174,49 +180,49 @@
     <t xml:space="preserve">sub_category</t>
   </si>
   <si>
+    <t xml:space="preserve">Off Premise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beer Tap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On Premise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stacking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">others</t>
+  </si>
+  <si>
+    <t xml:space="preserve">irrelevant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scene_types_to_include</t>
+  </si>
+  <si>
+    <t xml:space="preserve">categories_to_exclude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beer Tap Category</t>
+  </si>
+  <si>
     <t xml:space="preserve">DST_MANUFACTURER_BY_SCENE_TYPE_ASSORTMENT</t>
   </si>
   <si>
-    <t xml:space="preserve">Off Premise</t>
-  </si>
-  <si>
     <t xml:space="preserve">PRODUCT_PRESENCE_BY_SCENE_TYPE_ASSORTMENT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beer Tap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">On Premise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stacking Logic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Others Logic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Irrelevant Logic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Empty Logic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Category Exclude </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Include</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exclude</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beer Tap Category</t>
   </si>
 </sst>
 </file>
@@ -226,7 +232,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -248,8 +254,15 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -276,30 +289,54 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
+        <fgColor rgb="FFC5F9CB"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF69ABE"/>
+        <bgColor rgb="FFFF99FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC5C2F5"/>
+        <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF977D"/>
+        <bgColor rgb="FFF69ABE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE9F9E2"/>
+        <bgColor rgb="FFF8F8C9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8F8C9"/>
         <bgColor rgb="FFE9F9E2"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE9F9E2"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF66FF99"/>
-        <bgColor rgb="FF99CCFF"/>
+        <bgColor rgb="FFC5F9CB"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF99FF"/>
-        <bgColor rgb="FFCC99FF"/>
+        <bgColor rgb="FFF69ABE"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -312,13 +349,6 @@
       <right style="hair"/>
       <top style="hair"/>
       <bottom style="hair"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -347,7 +377,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -362,6 +392,18 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -392,27 +434,43 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -428,7 +486,7 @@
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFE9F9E2"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
@@ -445,12 +503,12 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFE9F9E2"/>
+      <rgbColor rgb="FFF8F8C9"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FFFF977D"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFC5C2F5"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -461,12 +519,12 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFFBF5A4"/>
+      <rgbColor rgb="FFC5F9CB"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFF69ABE"/>
       <rgbColor rgb="FFFF99FF"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFBF5A4"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF66FF99"/>
       <rgbColor rgb="FF99CC00"/>
@@ -496,17 +554,16 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E45" activeCellId="0" sqref="E45"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="1" sqref="A14:B17 C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.4438775510204"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="45.6275510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="66.3163265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.6530612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="42.3877551020408"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -516,130 +573,192 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>3</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3"/>
+      <c r="C3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="3"/>
+      <c r="C4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="3"/>
+      <c r="C5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="H5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B6" s="3"/>
+      <c r="C6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B7" s="3"/>
+      <c r="C7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B8" s="3"/>
-      <c r="H8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" s="5"/>
+      <c r="C8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="H8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B9" s="3"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="5"/>
+      <c r="C9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" s="5"/>
+        <v>15</v>
+      </c>
+      <c r="C10" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="H10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B11" s="3"/>
-      <c r="H11" s="4" t="s">
-        <v>16</v>
+      <c r="C11" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="H11" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="C12" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="H12" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B13" s="3"/>
-      <c r="H13" s="4" t="s">
-        <v>23</v>
+      <c r="C13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="H13" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>26</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B15" s="3"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B2:B9"/>
+    <mergeCell ref="H5:I6"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="B14:B15"/>
@@ -664,63 +783,70 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topRight" activeCell="A14" activeCellId="0" sqref="A14:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="63.984693877551"/>
-    <col collapsed="false" hidden="false" max="12" min="2" style="6" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="6" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="1023" min="14" style="6" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="9" width="66.3163265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="45.3214285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="9" width="12.7448979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="9" width="13.0561224489796"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="9" width="9.19897959183673"/>
+    <col collapsed="false" hidden="false" max="10" min="7" style="9" width="14.9030612244898"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="9" width="13.0561224489796"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="9" width="22.0102040816327"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="9" width="11.3571428571429"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="9" width="8.11734693877551"/>
+    <col collapsed="false" hidden="false" max="1023" min="16" style="9" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="7" t="s">
+      <c r="B1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="C1" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="D1" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="E1" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="F1" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="G1" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="H1" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="I1" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="J1" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="K1" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="L1" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="M1" s="11" t="s">
         <v>41</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>43</v>
       </c>
       <c r="P1" s="0"/>
       <c r="Q1" s="0"/>
@@ -1732,40 +1858,37 @@
       <c r="AMI1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="10" t="s">
+      <c r="A2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="0"/>
-      <c r="J2" s="0"/>
-      <c r="K2" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="M2" s="6" t="s">
+      <c r="D2" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="N2" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="O2" s="6" t="s">
+      <c r="E2" s="15"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="13" t="s">
         <v>46</v>
+      </c>
+      <c r="H2" s="14"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>48</v>
       </c>
       <c r="P2" s="0"/>
       <c r="Q2" s="0"/>
@@ -2777,36 +2900,38 @@
       <c r="AMI2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="10"/>
-      <c r="K3" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="M3" s="6" t="s">
+      <c r="A3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="N3" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>46</v>
+      <c r="E3" s="15"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="O3" s="9" t="s">
+        <v>48</v>
       </c>
       <c r="P3" s="0"/>
       <c r="Q3" s="0"/>
@@ -3818,365 +3943,398 @@
       <c r="AMI3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="10" t="s">
+      <c r="C4" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="16"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="M4" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="10"/>
-      <c r="K4" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="M4" s="6" t="s">
+      <c r="N4" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="N4" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>46</v>
+      <c r="O4" s="9" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="10" t="s">
+      <c r="C5" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="13"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="M5" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="N5" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="O5" s="9" t="s">
         <v>48</v>
-      </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="10"/>
-      <c r="K5" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="O5" s="6" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="10" t="s">
+      <c r="A6" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="17"/>
+      <c r="C6" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="10"/>
-      <c r="K6" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="O6" s="6" t="s">
+      <c r="D6" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="15"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="13" t="s">
         <v>46</v>
+      </c>
+      <c r="H6" s="14"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="O6" s="9" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="10"/>
-      <c r="K7" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="M7" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>46</v>
+      <c r="A7" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="15"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="M7" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="O7" s="9" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="A8" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="F8" s="16"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="M8" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="10"/>
-      <c r="K8" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="L8" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="M8" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="O8" s="6" t="s">
-        <v>46</v>
+      <c r="O8" s="9" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="F9" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="13"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="M9" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="O9" s="9" t="s">
         <v>48</v>
-      </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="10"/>
-      <c r="K9" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="M9" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="O9" s="6" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="10"/>
-      <c r="K10" s="6" t="s">
+      <c r="A10" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="15"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="M10" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="O10" s="9" t="s">
         <v>48</v>
-      </c>
-      <c r="L10" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="M10" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="O10" s="6" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="15"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="M11" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="10"/>
-      <c r="K11" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="L11" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="M11" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="O11" s="6" t="s">
+      <c r="O11" s="9" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="10"/>
-      <c r="K12" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="L12" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="M12" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="O12" s="6" t="s">
-        <v>46</v>
+      <c r="A12" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="15"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="O12" s="9" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="10"/>
-      <c r="K13" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="L13" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="M13" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="O13" s="6" t="s">
+      <c r="A13" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="15"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="L13" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="M13" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="O13" s="9" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="2" t="s">
+      <c r="A14" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="G14" s="2" t="s">
+      <c r="E14" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="16"/>
+      <c r="G14" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="H14" s="10"/>
-      <c r="K14" s="6" t="s">
+      <c r="I14" s="15"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="M14" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="O14" s="9" t="s">
         <v>48</v>
-      </c>
-      <c r="L14" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="M14" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="O14" s="6" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="A15" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="17"/>
+      <c r="C15" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="2" t="s">
+      <c r="E15" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="16"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="H15" s="10"/>
-      <c r="K15" s="6" t="s">
+      <c r="I15" s="15"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="M15" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="O15" s="9" t="s">
         <v>48</v>
-      </c>
-      <c r="L15" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="M15" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="O15" s="6" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -4195,314 +4353,364 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="1" sqref="A14:B17 G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="61.6887755102041"/>
-    <col collapsed="false" hidden="false" max="6" min="2" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="57.5051020408163"/>
+    <col collapsed="false" hidden="false" max="5" min="2" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="9" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="1" t="s">
         <v>61</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="D2" s="0" t="s">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>64</v>
-      </c>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" s="0" t="s">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="F3" s="0" t="s">
+      <c r="G3" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D4" s="15" t="s">
+      <c r="A4" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="F4" s="15" t="s">
+      <c r="G4" s="21" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="15" t="s">
+      <c r="A5" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5" s="15" t="s">
+      <c r="G5" s="21" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D6" s="15" t="s">
+      <c r="A6" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="E6" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="F6" s="15" t="s">
+      <c r="G6" s="21" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="15" t="s">
+      <c r="A7" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="E7" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="F7" s="15" t="s">
+      <c r="G7" s="21" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D8" s="15" t="s">
+      <c r="A8" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="E8" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="F8" s="15" t="s">
+      <c r="G8" s="21" t="s">
         <v>64</v>
       </c>
+      <c r="J8" s="22"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D9" s="15" t="s">
+      <c r="A9" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="F9" s="15" t="s">
+      <c r="G9" s="21" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10" s="15" t="s">
+      <c r="A10" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="E10" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="F10" s="15" t="s">
+      <c r="G10" s="21" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11" s="15" t="s">
+      <c r="A11" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="E11" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="F11" s="15" t="s">
+      <c r="G11" s="21" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D12" s="15" t="s">
+      <c r="A12" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="E12" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="F12" s="15" t="s">
+      <c r="G12" s="21" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D13" s="15" t="s">
+      <c r="A13" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="F13" s="15" t="s">
+      <c r="G13" s="21" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D14" s="15" t="s">
+      <c r="A14" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="E14" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="F14" s="15"/>
+      <c r="G14" s="21"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" s="15" t="s">
+      <c r="A15" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="E15" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="F15" s="15"/>
+      <c r="G15" s="21"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
adding irrelevant products for fsos
</commit_message>
<xml_diff>
--- a/Projects/LIONNZ/Data/Template.xlsx
+++ b/Projects/LIONNZ/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="kpis" sheetId="1" state="visible" r:id="rId2"/>
@@ -481,13 +481,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="60.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="4" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.1836734693878"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -636,7 +635,7 @@
   </sheetPr>
   <dimension ref="A1:AMH12"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C28" activeCellId="0" sqref="C28"/>
@@ -644,20 +643,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="47.3928571428572"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="67.9030612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="8" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="8" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="8" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="8" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="8" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="8" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="8" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="8" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="8" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="1022" min="15" style="8" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="45.7602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="65.6071428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="8" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="8" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="8" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="8" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="8" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="8" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="8" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="8" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="8" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="1022" min="15" style="8" width="7.29081632653061"/>
     <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="6.0765306122449"/>
   </cols>
   <sheetData>
@@ -5121,22 +5120,22 @@
   </sheetPr>
   <dimension ref="1:12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="15" width="53.5918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="15" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="15" width="57.5051020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="15" width="7.02040816326531"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="15" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="15" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="15" width="7.83163265306122"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="15" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="16" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="15" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="15" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="15" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="15" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="16" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="15" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="15" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="15" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="15" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" s="20" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5179,7 +5178,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>0</v>
@@ -6214,8 +6213,8 @@
       <c r="C3" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="D3" s="22" t="n">
-        <v>0</v>
+      <c r="D3" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="E3" s="22" t="n">
         <v>0</v>
@@ -6236,8 +6235,8 @@
       <c r="C4" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="D4" s="22" t="n">
-        <v>0</v>
+      <c r="D4" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="E4" s="22" t="n">
         <v>0</v>
@@ -6258,8 +6257,8 @@
       <c r="C5" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="22" t="n">
-        <v>0</v>
+      <c r="D5" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="E5" s="22" t="n">
         <v>0</v>
@@ -6280,8 +6279,8 @@
       <c r="C6" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="D6" s="22" t="n">
-        <v>0</v>
+      <c r="D6" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="E6" s="22" t="n">
         <v>0</v>
@@ -6302,8 +6301,8 @@
       <c r="C7" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="D7" s="22" t="n">
-        <v>0</v>
+      <c r="D7" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="E7" s="22" t="n">
         <v>0</v>
@@ -6324,8 +6323,8 @@
       <c r="C8" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="D8" s="22" t="n">
-        <v>0</v>
+      <c r="D8" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="E8" s="22" t="n">
         <v>0</v>
@@ -6346,8 +6345,8 @@
       <c r="C9" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="D9" s="22" t="n">
-        <v>0</v>
+      <c r="D9" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="E9" s="22" t="n">
         <v>0</v>
@@ -6368,8 +6367,8 @@
       <c r="C10" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="D10" s="22" t="n">
-        <v>0</v>
+      <c r="D10" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="E10" s="22" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
showing scene/category for own manuf even if zero
</commit_message>
<xml_diff>
--- a/Projects/LIONNZ/Data/Template.xlsx
+++ b/Projects/LIONNZ/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="kpis" sheetId="1" state="visible" r:id="rId2"/>
@@ -481,12 +481,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.1836734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="4" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="57.5051020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -635,29 +635,25 @@
   </sheetPr>
   <dimension ref="A1:AMH12"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C28" activeCellId="0" sqref="C28"/>
+      <selection pane="topRight" activeCell="L7" activeCellId="0" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="45.7602040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="65.6071428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="8" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="8" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="8" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="8" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="8" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="8" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="8" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="8" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="8" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="1022" min="15" style="8" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="46.8673469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="66.3163265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="12.7448979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="11.3571428571429"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="8" width="9.19897959183673"/>
+    <col collapsed="false" hidden="false" max="10" min="7" style="8" width="14.9030612244898"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="8" width="12.7448979591837"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="8" width="21.0867346938776"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="8" width="12.7448979591837"/>
+    <col collapsed="false" hidden="false" max="1022" min="15" style="8" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2774,7 +2770,7 @@
       <c r="K3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L3" s="1" t="s">
         <v>34</v>
       </c>
       <c r="M3" s="7" t="s">
@@ -4924,7 +4920,7 @@
       <c r="K7" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="L7" s="6" t="s">
+      <c r="L7" s="1" t="s">
         <v>37</v>
       </c>
       <c r="M7" s="7" t="s">
@@ -5120,22 +5116,22 @@
   </sheetPr>
   <dimension ref="1:12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="15" width="57.5051020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="15" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="15" width="56.8316326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="15" width="6.88265306122449"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="15" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="15" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="15" width="7.69387755102041"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="15" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="16" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="15" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="15" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="15" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="15" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="16" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="15" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="15" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="15" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="15" width="7.96428571428571"/>
   </cols>
   <sheetData>
     <row r="1" s="20" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
adding irrelevant, extra own manufacturer
</commit_message>
<xml_diff>
--- a/Projects/LIONNZ/Data/Template.xlsx
+++ b/Projects/LIONNZ/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="kpis" sheetId="1" state="visible" r:id="rId2"/>
@@ -481,11 +481,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="56.8316326530612"/>
-    <col collapsed="false" hidden="false" max="7" min="4" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="56.1581632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.3775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -634,7 +633,7 @@
   </sheetPr>
   <dimension ref="A1:AMH12"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="L13" activeCellId="0" sqref="L13"/>
@@ -642,17 +641,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="46.3010204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="65.469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="8" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="10" min="7" style="8" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="8" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="8" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="8" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1022" min="15" style="8" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="45.7602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="64.6632653061225"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="8" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="10" min="7" style="8" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="8" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="8" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="8" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1022" min="15" style="8" width="11.0714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5115,22 +5113,22 @@
   </sheetPr>
   <dimension ref="1:12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F33" activeCellId="0" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="15" width="56.1581632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="15" width="6.75"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="15" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="15" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="15" width="55.4795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="15" width="8.5765306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="15" width="6.87755102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="15" width="9.50510204081633"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="15" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="16" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="15" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="15" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="15" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="15" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="16" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="15" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="15" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="15" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="15" width="7.69387755102041"/>
   </cols>
   <sheetData>
     <row r="1" s="20" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5173,7 +5171,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>0</v>
@@ -6208,8 +6206,8 @@
       <c r="C3" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="D3" s="0" t="n">
-        <v>1</v>
+      <c r="D3" s="22" t="n">
+        <v>0</v>
       </c>
       <c r="E3" s="22" t="n">
         <v>0</v>
@@ -6230,8 +6228,8 @@
       <c r="C4" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="D4" s="0" t="n">
-        <v>1</v>
+      <c r="D4" s="22" t="n">
+        <v>0</v>
       </c>
       <c r="E4" s="22" t="n">
         <v>0</v>
@@ -6252,8 +6250,8 @@
       <c r="C5" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="0" t="n">
-        <v>1</v>
+      <c r="D5" s="22" t="n">
+        <v>0</v>
       </c>
       <c r="E5" s="22" t="n">
         <v>0</v>
@@ -6274,8 +6272,8 @@
       <c r="C6" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="D6" s="0" t="n">
-        <v>1</v>
+      <c r="D6" s="22" t="n">
+        <v>0</v>
       </c>
       <c r="E6" s="22" t="n">
         <v>0</v>
@@ -6296,8 +6294,8 @@
       <c r="C7" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="D7" s="0" t="n">
-        <v>1</v>
+      <c r="D7" s="22" t="n">
+        <v>0</v>
       </c>
       <c r="E7" s="22" t="n">
         <v>0</v>
@@ -6318,8 +6316,8 @@
       <c r="C8" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="D8" s="0" t="n">
-        <v>1</v>
+      <c r="D8" s="22" t="n">
+        <v>0</v>
       </c>
       <c r="E8" s="22" t="n">
         <v>0</v>
@@ -6340,8 +6338,8 @@
       <c r="C9" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="D9" s="0" t="n">
-        <v>1</v>
+      <c r="D9" s="22" t="n">
+        <v>0</v>
       </c>
       <c r="E9" s="22" t="n">
         <v>0</v>
@@ -6362,8 +6360,8 @@
       <c r="C10" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="D10" s="0" t="n">
-        <v>1</v>
+      <c r="D10" s="22" t="n">
+        <v>0</v>
       </c>
       <c r="E10" s="22" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
fix bug- not showing when categ is zero
</commit_message>
<xml_diff>
--- a/Projects/LIONNZ/Data/Template.xlsx
+++ b/Projects/LIONNZ/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="kpis" sheetId="1" state="visible" r:id="rId2"/>
@@ -476,17 +476,16 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="N3 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.4795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="4" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -635,25 +634,25 @@
   </sheetPr>
   <dimension ref="A1:AMH12"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="L13" activeCellId="0" sqref="L13"/>
+      <selection pane="topRight" activeCell="N3" activeCellId="0" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="45.2244897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="63.984693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="8" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="7" style="8" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="8" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="8" width="20.25"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="8" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="1022" min="15" style="8" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="44.1428571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="62.5"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="8" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="10" min="7" style="8" width="13.5"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="8" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="8" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="8" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1022" min="15" style="8" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2777,7 +2776,7 @@
         <v>33</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="O3" s="0"/>
       <c r="P3" s="0"/>
@@ -5116,22 +5115,22 @@
   </sheetPr>
   <dimension ref="1:12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="1" sqref="N3 D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="15" width="54.8061224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="15" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="15" width="6.75"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="15" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="15" width="53.5918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="15" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="15" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="15" width="9.17857142857143"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="15" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="16" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="15" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="15" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="15" width="20.25"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="15" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="16" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="15" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="15" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="15" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="15" width="7.29081632653061"/>
   </cols>
   <sheetData>
     <row r="1" s="20" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
PROS-12633 - Change Beer Tap to Tap
</commit_message>
<xml_diff>
--- a/Projects/LIONNZ/Data/Template.xlsx
+++ b/Projects/LIONNZ/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="kpis" sheetId="1" state="visible" r:id="rId2"/>
@@ -138,7 +138,7 @@
     <t xml:space="preserve">category</t>
   </si>
   <si>
-    <t xml:space="preserve">Beer Tap</t>
+    <t xml:space="preserve">Tap</t>
   </si>
   <si>
     <t xml:space="preserve">on premise</t>
@@ -475,17 +475,18 @@
   </sheetPr>
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="N3 B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.265306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="4" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.23469387755102"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="54.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="24.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -619,7 +620,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -634,25 +635,25 @@
   </sheetPr>
   <dimension ref="A1:AMH12"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="N3" activeCellId="0" sqref="N3"/>
+      <selection pane="topRight" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="44.1428571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="62.5"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="8" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="10" min="7" style="8" width="13.5"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="8" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="8" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="8" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="1022" min="15" style="8" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.23469387755102"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="44.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="62.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="11.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="8" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="8" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="7" style="8" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="8" width="11.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="8" width="19.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="8" width="11.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="15" style="8" width="10.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="8.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5100,7 +5101,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -5113,24 +5114,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:12"/>
+  <dimension ref="A1:AMJ12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="1" sqref="N3 D7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="15" width="53.5918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="15" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="15" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="15" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="15" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="16" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="15" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="15" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="15" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="15" width="7.29081632653061"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="15" width="53.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="15" width="8.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="15" width="6.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="15" width="9.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="15" width="6.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="16" width="16.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="15" width="17.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="15" width="16.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="15" width="19.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="15" width="7.29"/>
   </cols>
   <sheetData>
     <row r="1" s="20" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6418,7 +6419,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
fixing the tap category
</commit_message>
<xml_diff>
--- a/Projects/LIONNZ/Data/Template.xlsx
+++ b/Projects/LIONNZ/Data/Template.xlsx
@@ -138,7 +138,7 @@
     <t xml:space="preserve">category</t>
   </si>
   <si>
-    <t xml:space="preserve">Beer Tap</t>
+    <t xml:space="preserve">Tap</t>
   </si>
   <si>
     <t xml:space="preserve">on premise</t>
@@ -476,16 +476,15 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="N3 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.265306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="4" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.5918367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.3010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -637,22 +636,22 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="N3" activeCellId="0" sqref="N3"/>
+      <selection pane="topRight" activeCell="E31" activeCellId="0" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="44.1428571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="62.5"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="8" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="10" min="7" style="8" width="13.5"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="8" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="8" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="8" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="1022" min="15" style="8" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="43.6020408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="61.6887755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="8" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="10" min="7" style="8" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="8" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="8" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="8" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="1022" min="15" style="8" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5116,21 +5115,21 @@
   <dimension ref="1:12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="1" sqref="N3 D7"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="15" width="53.5918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="15" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="15" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="15" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="15" width="52.9183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="15" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="15" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="15" width="9.04591836734694"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="15" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="16" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="15" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="15" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="15" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="15" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="16" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="15" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="15" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="15" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="15" width="7.1530612244898"/>
   </cols>
   <sheetData>
     <row r="1" s="20" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>